<commit_message>
Corrigiendo faltas de ortografia
</commit_message>
<xml_diff>
--- a/info/INVENTARIO EQUIPOS ESCANEO.xlsx
+++ b/info/INVENTARIO EQUIPOS ESCANEO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="72">
   <si>
     <t>EQUIPOS ESCANEO CDA</t>
   </si>
@@ -231,13 +231,22 @@
   </si>
   <si>
     <t>ESCANER KOICA</t>
+  </si>
+  <si>
+    <t>I5 8RAM 512GB</t>
+  </si>
+  <si>
+    <t>MATRIZ</t>
+  </si>
+  <si>
+    <t>LAPTOP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,6 +258,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -578,102 +594,129 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -954,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="M17" sqref="K17:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,583 +1009,690 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="27.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="5" max="6" width="27.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="16" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="17"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="9" t="s">
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+      <c r="M3" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="22">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="25">
         <v>27994870</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="35">
+        <v>101</v>
+      </c>
+      <c r="G4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="H4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="I4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="30">
+      <c r="J4" s="25">
         <v>13823697</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="K4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="30" t="s">
+      <c r="L4" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="M4" s="36">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="29">
         <v>27995641</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="35">
+        <v>102</v>
+      </c>
+      <c r="G5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="12">
+      <c r="J5" s="29">
         <v>13822719</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="M5" s="36">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="22">
         <v>3</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="25">
         <v>27994190</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="35">
+        <v>103</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="H6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="I6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="30">
+      <c r="J6" s="25">
         <v>13822581</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="K6" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="L6" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="M6" s="36">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="29">
         <v>27994864</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="35">
+        <v>104</v>
+      </c>
+      <c r="G7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="12">
+      <c r="J7" s="29">
         <v>13823592</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+      <c r="M7" s="36">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="22">
         <v>5</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="25">
         <v>27995761</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="35">
+        <v>105</v>
+      </c>
+      <c r="G8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="H8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="I8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="30">
+      <c r="J8" s="25">
         <v>13823604</v>
       </c>
-      <c r="J8" s="28" t="s">
+      <c r="K8" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="30" t="s">
+      <c r="L8" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="M8" s="36">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="29">
         <v>27994560</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="35">
+        <v>106</v>
+      </c>
+      <c r="G9" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="H9" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="12">
+      <c r="J9" s="29">
         <v>13822906</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="L9" s="29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="M9" s="36">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
         <v>7</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="25">
         <v>27994553</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="35">
+        <v>107</v>
+      </c>
+      <c r="G10" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="H10" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="I10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="30">
+      <c r="J10" s="25">
         <v>13823658</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="K10" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="L10" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="M10" s="36">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="29">
         <v>27995277</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="35">
+        <v>108</v>
+      </c>
+      <c r="G11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="12">
+      <c r="J11" s="29">
         <v>13824214</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+      <c r="M11" s="36">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="22">
         <v>9</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="25">
         <v>27994517</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="35">
+        <v>109</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="H12" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="I12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="30">
+      <c r="J12" s="25">
         <v>13822651</v>
       </c>
-      <c r="J12" s="28" t="s">
+      <c r="K12" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="L12" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="M12" s="36">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="29">
         <v>27995768</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="35">
+        <v>110</v>
+      </c>
+      <c r="G13" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="H13" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="12">
+      <c r="J13" s="29">
         <v>13823925</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="K13" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="L13" s="29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="27">
+      <c r="M13" s="36">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="22">
         <v>11</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="25">
         <v>27995396</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="35">
+        <v>111</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="H14" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="I14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="30">
+      <c r="J14" s="25">
         <v>13823909</v>
       </c>
-      <c r="J14" s="28" t="s">
+      <c r="K14" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="30" t="s">
+      <c r="L14" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="M14" s="36">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>12</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="29">
         <v>27994605</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="35">
+        <v>112</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="H15" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="12">
+      <c r="J15" s="29">
         <v>13823875</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="K15" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="L15" s="29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+      <c r="M15" s="36">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
         <v>13</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="25">
         <v>27994127</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="35">
+        <v>113</v>
+      </c>
+      <c r="G16" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="H16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="I16" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="30">
+      <c r="J16" s="25">
         <v>13822989</v>
       </c>
-      <c r="J16" s="28" t="s">
+      <c r="K16" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="K16" s="30" t="s">
+      <c r="L16" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="M16" s="36">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="32">
         <v>27995335</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="35">
+        <v>114</v>
+      </c>
+      <c r="G17" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="H17" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="I17" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="15">
+      <c r="J17" s="32">
         <v>13823321</v>
       </c>
-      <c r="J17" s="13" t="s">
+      <c r="K17" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="L17" s="32" t="s">
         <v>7</v>
+      </c>
+      <c r="M17" s="36">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:L1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="E2:G2"/>
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>